<commit_message>
replaced TVS diodes by diodes with higher breakdown voltage to minimize leakage current
</commit_message>
<xml_diff>
--- a/Production Files/Rev_B/Solaranlage_Rev.B.xlsx
+++ b/Production Files/Rev_B/Solaranlage_Rev.B.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mstof\source\repos\solaranlage\Production Files\Rev_B\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B14080A2-AFD8-4F18-A9C4-7DE0D7BD5594}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{981BAEBC-3017-4C38-B9EC-A496CABD0E56}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -85,9 +85,6 @@
     <t>D8 D9 D10 D11 D14</t>
   </si>
   <si>
-    <t>140823-62 140823 - 62</t>
-  </si>
-  <si>
     <t>Light emitting diode</t>
   </si>
   <si>
@@ -443,6 +440,9 @@
   </si>
   <si>
     <t>739443-62 / MPE 087-1-020</t>
+  </si>
+  <si>
+    <t>140810-62</t>
   </si>
 </sst>
 </file>
@@ -1302,7 +1302,7 @@
   <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="B7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1317,10 +1317,10 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>112</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>113</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
@@ -1369,7 +1369,7 @@
         <v>8</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>9</v>
@@ -1389,7 +1389,7 @@
         <v>8</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>9</v>
@@ -1400,7 +1400,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>14</v>
@@ -1409,7 +1409,7 @@
         <v>8</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>9</v>
@@ -1429,7 +1429,7 @@
         <v>8</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>15</v>
@@ -1449,10 +1449,10 @@
         <v>8</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>20</v>
+        <v>139</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1460,19 +1460,19 @@
         <v>2</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="D8" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1480,19 +1480,19 @@
         <v>1</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="D9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1500,19 +1500,19 @@
         <v>6</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="F10" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1520,19 +1520,19 @@
         <v>1</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="F11" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1540,19 +1540,19 @@
         <v>1</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="F12" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1560,19 +1560,19 @@
         <v>3</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1580,19 +1580,19 @@
         <v>1</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1600,16 +1600,16 @@
         <v>2</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1617,19 +1617,19 @@
         <v>1</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1637,19 +1637,19 @@
         <v>3</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="F17" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1657,16 +1657,16 @@
         <v>1</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1674,16 +1674,16 @@
         <v>2</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1691,16 +1691,16 @@
         <v>1</v>
       </c>
       <c r="B20" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1708,16 +1708,16 @@
         <v>1</v>
       </c>
       <c r="B21" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>60</v>
-      </c>
       <c r="D21" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1725,19 +1725,19 @@
         <v>2</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1745,19 +1745,19 @@
         <v>8</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C23" s="2">
         <v>220</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1765,19 +1765,19 @@
         <v>6</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C24" s="2">
         <v>330</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1785,19 +1785,19 @@
         <v>3</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C25" s="2">
         <v>560</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1805,19 +1805,19 @@
         <v>8</v>
       </c>
       <c r="B26" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="D26" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1825,19 +1825,19 @@
         <v>1</v>
       </c>
       <c r="B27" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="D27" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1845,19 +1845,19 @@
         <v>9</v>
       </c>
       <c r="B28" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="D28" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1865,19 +1865,19 @@
         <v>2</v>
       </c>
       <c r="B29" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>76</v>
-      </c>
       <c r="F29" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1885,19 +1885,19 @@
         <v>1</v>
       </c>
       <c r="B30" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="D30" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>80</v>
-      </c>
       <c r="F30" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1905,19 +1905,19 @@
         <v>1</v>
       </c>
       <c r="B31" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>83</v>
-      </c>
       <c r="F31" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1925,19 +1925,19 @@
         <v>1</v>
       </c>
       <c r="B32" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>87</v>
-      </c>
       <c r="F32" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1945,19 +1945,19 @@
         <v>1</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D33" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="F33" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1965,19 +1965,19 @@
         <v>1</v>
       </c>
       <c r="B34" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>94</v>
-      </c>
       <c r="F34" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1985,19 +1985,19 @@
         <v>1</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -2005,19 +2005,19 @@
         <v>1</v>
       </c>
       <c r="B36" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="D36" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="F36" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -2025,19 +2025,19 @@
         <v>1</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -2045,19 +2045,19 @@
         <v>6</v>
       </c>
       <c r="B38" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="D38" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>108</v>
-      </c>
       <c r="F38" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -2065,19 +2065,19 @@
         <v>1</v>
       </c>
       <c r="B39" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>111</v>
-      </c>
       <c r="D39" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="53" spans="6:6" x14ac:dyDescent="0.25">

</xml_diff>